<commit_message>
Documentation effort part 2
</commit_message>
<xml_diff>
--- a/documentation/endpoints.xlsx
+++ b/documentation/endpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dearo\work\da-vinci\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFB57F8-3CE2-4BBA-8D1E-B6539B0623B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8367E3-FA4F-434F-A060-4F1BE69953AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20175" yWindow="1500" windowWidth="22830" windowHeight="20295" xr2:uid="{5E7EB52F-3B44-4EFB-95CE-434321CE891A}"/>
+    <workbookView xWindow="17865" yWindow="1515" windowWidth="35550" windowHeight="20295" xr2:uid="{5E7EB52F-3B44-4EFB-95CE-434321CE891A}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="72">
   <si>
     <t xml:space="preserve">Végpont </t>
   </si>
@@ -134,13 +134,130 @@
   </si>
   <si>
     <t>Listában tartalmazza minden futó asztalról a választott játék címét,csatlakozott játékos neveit, az asztal azonosítóját, hozzá adott gépi ellenfelek számát és hogy lehet e csatlakozni még az asztalhoz.</t>
+  </si>
+  <si>
+    <t>Topik neve</t>
+  </si>
+  <si>
+    <t>Küldő fél</t>
+  </si>
+  <si>
+    <t>Fogadó fél</t>
+  </si>
+  <si>
+    <t>Küldött adat</t>
+  </si>
+  <si>
+    <t>Megjegyzés</t>
+  </si>
+  <si>
+    <t>user-connected</t>
+  </si>
+  <si>
+    <t>game-init</t>
+  </si>
+  <si>
+    <t>public-hand-update</t>
+  </si>
+  <si>
+    <t>private-hand-update</t>
+  </si>
+  <si>
+    <t>message-info</t>
+  </si>
+  <si>
+    <t>guess</t>
+  </si>
+  <si>
+    <t>pick-color</t>
+  </si>
+  <si>
+    <t>take-extra-action</t>
+  </si>
+  <si>
+    <t>game-over</t>
+  </si>
+  <si>
+    <t>kliens</t>
+  </si>
+  <si>
+    <t>szerver</t>
+  </si>
+  <si>
+    <t>SetupInfo</t>
+  </si>
+  <si>
+    <t>PublicHand</t>
+  </si>
+  <si>
+    <t>GamePiece lista</t>
+  </si>
+  <si>
+    <t>A szerver kéri a klienst a jelzett akció végrehajtására.</t>
+  </si>
+  <si>
+    <t>Választható színek listája</t>
+  </si>
+  <si>
+    <t>Választható extra akciók listája</t>
+  </si>
+  <si>
+    <t>Nyertes játékos neve</t>
+  </si>
+  <si>
+    <t>Választott szín</t>
+  </si>
+  <si>
+    <t>Játékos által tett tipp</t>
+  </si>
+  <si>
+    <t>Választott extra akció</t>
+  </si>
+  <si>
+    <t>A kliens válaszol a szerver által kért akcióval.</t>
+  </si>
+  <si>
+    <t>Ellenfelek kódsorai, amely elemek publikusak azok értékkel is el vannak látva.</t>
+  </si>
+  <si>
+    <t>Saját kódsorunk legfrissebb állapota.</t>
+  </si>
+  <si>
+    <t>Rendszer üzenet</t>
+  </si>
+  <si>
+    <t>Szerver által küldött üzenet a játék állapotával kapcsolatban.</t>
+  </si>
+  <si>
+    <t>A küldött adat tartalmazza a játékosok neveit és a játék beállításait.</t>
+  </si>
+  <si>
+    <t>A kliens válaszol a szerver által kért akcióval (A felhasználó reagált a játék vége feliratra.)</t>
+  </si>
+  <si>
+    <t>table-list</t>
+  </si>
+  <si>
+    <t>server-start</t>
+  </si>
+  <si>
+    <t>Aktuális asztalok listája</t>
+  </si>
+  <si>
+    <t>Esetleges kliens újra csatlakozás esetén így jelzi a kliens a szerver felé, hogy már képes folytatni a játékot.</t>
+  </si>
+  <si>
+    <t>Ha a szerveren változik a futtatott asztalok állapot, a kliensek e módon tudnak róla értesülni.</t>
+  </si>
+  <si>
+    <t>Esetleges szerver újra indulás esetén tud a kliens reagálni egy oldal újratöltéssel.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -182,8 +299,23 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -214,6 +346,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -227,7 +377,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -276,12 +426,131 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <i/>
+        <charset val="238"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+        <charset val="238"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <i/>
+        <charset val="238"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="0" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <i/>
@@ -320,6 +589,9 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" relativeIndent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -333,9 +605,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -356,14 +625,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2D21CA4E-C3EA-4A14-96E0-F34944F53D80}" name="Táblázat3" displayName="Táblázat3" ref="B4:F16" totalsRowShown="0" headerRowDxfId="5" dataDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{2D21CA4E-C3EA-4A14-96E0-F34944F53D80}" name="Táblázat3" displayName="Táblázat3" ref="B4:F16" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
   <autoFilter ref="B4:F16" xr:uid="{2D21CA4E-C3EA-4A14-96E0-F34944F53D80}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{9C37B07A-43F6-489C-AF45-A94A52EBC0DD}" name="Végpont " dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{61C18667-807F-4846-A968-C62AF7D8BA3B}" name="Rest metódus" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{CB031264-A40B-42DF-A72B-AE34AA2F302D}" name="Várt adat" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{8D152250-BBC6-4966-9E49-C8C211B0F1C4}" name="Válasz adat" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{DA4CDAA2-9357-4253-8320-E9BAE2AC4595}" name="Megjegyzések" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{9C37B07A-43F6-489C-AF45-A94A52EBC0DD}" name="Végpont " dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{61C18667-807F-4846-A968-C62AF7D8BA3B}" name="Rest metódus" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{CB031264-A40B-42DF-A72B-AE34AA2F302D}" name="Várt adat" dataDxfId="9"/>
+    <tableColumn id="4" xr3:uid="{8D152250-BBC6-4966-9E49-C8C211B0F1C4}" name="Válasz adat" dataDxfId="8"/>
+    <tableColumn id="5" xr3:uid="{DA4CDAA2-9357-4253-8320-E9BAE2AC4595}" name="Megjegyzések" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{0E06AFF0-760E-4C4E-A6D5-0E4A35DA255D}" name="Táblázat2" displayName="Táblázat2" ref="I22:M37" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+  <autoFilter ref="I22:M37" xr:uid="{0E06AFF0-760E-4C4E-A6D5-0E4A35DA255D}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{EF80FE3D-8731-4E2B-A11F-7729F3FD26DD}" name="Topik neve" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{DA4BB459-79C2-439D-AD0E-4D20E97AA144}" name="Küldő fél" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{CE4E8D86-7A21-4893-857E-63180958D26D}" name="Fogadó fél" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{640CF15D-900F-4773-9F0D-F3647C993CD7}" name="Küldött adat" dataDxfId="1"/>
+    <tableColumn id="5" xr3:uid="{A414CC32-2689-4292-861F-4642C16B423D}" name="Megjegyzés" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -666,10 +949,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA38187-D0D0-4FE9-AD5E-651967619752}">
-  <dimension ref="B4:F16"/>
+  <dimension ref="B4:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="G13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P28" sqref="P28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -679,9 +962,14 @@
     <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.5703125" customWidth="1"/>
     <col min="6" max="6" width="44.28515625" customWidth="1"/>
+    <col min="9" max="9" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="30" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="96.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:6" ht="42" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:6" ht="21" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -902,11 +1190,284 @@
         <v>31</v>
       </c>
     </row>
+    <row r="22" spans="9:13" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I22" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="J22" s="20" t="s">
+        <v>34</v>
+      </c>
+      <c r="K22" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="L22" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="M22" s="20" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="9:13" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I23" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="J23" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="K23" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="L23" s="32" t="s">
+        <v>68</v>
+      </c>
+      <c r="M23" s="32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="24" spans="9:13" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I24" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="J24" s="34" t="s">
+        <v>48</v>
+      </c>
+      <c r="K24" s="34" t="s">
+        <v>47</v>
+      </c>
+      <c r="L24" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="M24" s="35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="9:13" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I25" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="J25" s="36" t="s">
+        <v>47</v>
+      </c>
+      <c r="K25" s="36" t="s">
+        <v>48</v>
+      </c>
+      <c r="L25" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="M25" s="32" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="9:13" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I26" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="J26" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="K26" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="L26" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="M26" s="27" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="9:13" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I27" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="J27" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="K27" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="L27" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="M27" s="27" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="9:13" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I28" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="J28" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="K28" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="L28" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="M28" s="27" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="29" spans="9:13" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I29" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="J29" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="K29" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="L29" s="17" t="s">
+        <v>62</v>
+      </c>
+      <c r="M29" s="27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="9:13" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I30" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="J30" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="K30" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="L30" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="M30" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="31" spans="9:13" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I31" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="J31" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="K31" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="L31" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="M31" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="9:13" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I32" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="J32" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="K32" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="L32" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="M32" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="33" spans="9:13" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I33" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="J33" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="K33" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="L33" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="M33" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="9:13" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I34" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="J34" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="K34" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="L34" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="M34" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="35" spans="9:13" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I35" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J35" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="K35" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="L35" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="M35" s="28" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="36" spans="9:13" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I36" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="J36" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="K36" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="L36" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="M36" s="29" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="9:13" s="17" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I37" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="J37" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="K37" s="24" t="s">
+        <v>48</v>
+      </c>
+      <c r="L37" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="M37" s="28" t="s">
+        <v>65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Documentation effort part 3
</commit_message>
<xml_diff>
--- a/documentation/endpoints.xlsx
+++ b/documentation/endpoints.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dearo\work\da-vinci\documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F8367E3-FA4F-434F-A060-4F1BE69953AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4508508-5B3F-4C5F-9097-A053421661A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17865" yWindow="1515" windowWidth="35550" windowHeight="20295" xr2:uid="{5E7EB52F-3B44-4EFB-95CE-434321CE891A}"/>
+    <workbookView xWindow="21765" yWindow="1395" windowWidth="25440" windowHeight="20640" xr2:uid="{5E7EB52F-3B44-4EFB-95CE-434321CE891A}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -951,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EA38187-D0D0-4FE9-AD5E-651967619752}">
   <dimension ref="B4:M37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView tabSelected="1" topLeftCell="G19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L41" sqref="L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>